<commit_message>
Update HQ (including graphs) to reflect change in MAX_DIST units
</commit_message>
<xml_diff>
--- a/source/en/habitat_quality/HQ-decay-functions-chart.xlsx
+++ b/source/en/habitat_quality/HQ-decay-functions-chart.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ddenu\Workspace\NatCap\Repositories\invest.users-guide\source\habitat_quality\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/eadavis/source/natcap/invest.users-guide/source/en/habitat_quality/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A21BBF9B-A4CE-49EF-8256-BC158A88B379}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE7329BE-F11C-234E-A8B1-3B39558AE0E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14476" xr2:uid="{350C4C21-B092-4F87-8388-43652A6CC636}"/>
+    <workbookView xWindow="34660" yWindow="500" windowWidth="31580" windowHeight="19880" xr2:uid="{350C4C21-B092-4F87-8388-43652A6CC636}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
@@ -133,7 +133,7 @@
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
-            <c:v>1 km</c:v>
+            <c:v>1000 m</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="19050" cap="rnd">
@@ -782,7 +782,7 @@
           <c:idx val="1"/>
           <c:order val="1"/>
           <c:tx>
-            <c:v>2 km</c:v>
+            <c:v>2000 m</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="19050" cap="rnd">
@@ -1431,7 +1431,7 @@
           <c:idx val="2"/>
           <c:order val="2"/>
           <c:tx>
-            <c:v>3 km</c:v>
+            <c:v>3000 m</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="19050" cap="rnd">
@@ -2080,7 +2080,7 @@
           <c:idx val="3"/>
           <c:order val="3"/>
           <c:tx>
-            <c:v>4 km</c:v>
+            <c:v>4000 m</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="19050" cap="rnd">
@@ -2731,7 +2731,7 @@
           <c:idx val="4"/>
           <c:order val="4"/>
           <c:tx>
-            <c:v>5 km</c:v>
+            <c:v>5000 m</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="19050" cap="rnd">
@@ -3600,16 +3600,13 @@
                   <a:buFontTx/>
                   <a:buNone/>
                   <a:tabLst/>
-                  <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="1400">
                     <a:solidFill>
                       <a:sysClr val="windowText" lastClr="000000">
                         <a:lumMod val="65000"/>
                         <a:lumOff val="35000"/>
                       </a:sysClr>
                     </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
                   </a:defRPr>
                 </a:pPr>
                 <a:endParaRPr lang="en-US" sz="1400"/>
@@ -4484,9 +4481,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -4524,7 +4521,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -4630,7 +4627,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -4772,7 +4769,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -4782,17 +4779,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B0294C04-675B-44C3-B97B-6F83172E938E}">
   <dimension ref="A1:C507"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="P15" sqref="P15"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="Q20" sqref="Q20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="14.3984375" customWidth="1"/>
-    <col min="3" max="3" width="31.06640625" customWidth="1"/>
+    <col min="1" max="1" width="14.33203125" customWidth="1"/>
+    <col min="3" max="3" width="31" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -4803,7 +4800,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1000</v>
       </c>
@@ -4815,7 +4812,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1000</v>
       </c>
@@ -4827,7 +4824,7 @@
         <v>0.86113843801970102</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>1000</v>
       </c>
@@ -4839,7 +4836,7 @@
         <v>0.74155940943501053</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>1000</v>
       </c>
@@ -4851,7 +4848,7 @@
         <v>0.6385853115396769</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>1000</v>
       </c>
@@ -4863,7 +4860,7 @@
         <v>0.54991035772160157</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>1000</v>
       </c>
@@ -4875,7 +4872,7 @@
         <v>0.47354894649923496</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>1000</v>
       </c>
@@ -4887,7 +4884,7 @@
         <v>0.4077912001142262</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>1000</v>
       </c>
@@ -4899,7 +4896,7 @@
         <v>0.35116467710454408</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>1000</v>
       </c>
@@ -4911,7 +4908,7 @@
         <v>0.30240140152949979</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>1000</v>
       </c>
@@ -4923,7 +4920,7 @@
         <v>0.26040947056808189</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>1000</v>
       </c>
@@ -4935,7 +4932,7 @@
         <v>0.22424860473053532</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>1000</v>
       </c>
@@ -4947,7 +4944,7 @@
         <v>0.19310909320575054</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>1000</v>
       </c>
@@ -4959,7 +4956,7 @@
         <v>0.16629366289060088</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>1000</v>
       </c>
@@ -4971,7 +4968,7 @@
         <v>0.14320186511418675</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>1000</v>
       </c>
@@ -4983,7 +4980,7 @@
         <v>0.12331663044593871</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>1000</v>
       </c>
@@ -4995,7 +4992,7 @@
         <v>0.10619269052406835</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>1000</v>
       </c>
@@ -5007,7 +5004,7 @@
         <v>9.1446607647005754E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>1000</v>
       </c>
@@ -5019,7 +5016,7 @@
         <v>7.8748188871342967E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>1000</v>
       </c>
@@ -5031,7 +5028,7 @@
         <v>6.7813092361548713E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>1000</v>
       </c>
@@ -5043,7 +5040,7 @@
         <v>5.8396460433509767E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>1000</v>
       </c>
@@ -5055,7 +5052,7 @@
         <v>5.0287436723591865E-2</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>1000</v>
       </c>
@@ -5066,7 +5063,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>1000</v>
       </c>
@@ -5077,7 +5074,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>1000</v>
       </c>
@@ -5088,7 +5085,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>1000</v>
       </c>
@@ -5099,7 +5096,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>1000</v>
       </c>
@@ -5110,7 +5107,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>1000</v>
       </c>
@@ -5121,7 +5118,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>1000</v>
       </c>
@@ -5132,7 +5129,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>1000</v>
       </c>
@@ -5143,7 +5140,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>1000</v>
       </c>
@@ -5154,7 +5151,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>1000</v>
       </c>
@@ -5165,7 +5162,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>1000</v>
       </c>
@@ -5176,7 +5173,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>1000</v>
       </c>
@@ -5187,7 +5184,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>1000</v>
       </c>
@@ -5198,7 +5195,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>1000</v>
       </c>
@@ -5209,7 +5206,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>1000</v>
       </c>
@@ -5220,7 +5217,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>1000</v>
       </c>
@@ -5231,7 +5228,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>1000</v>
       </c>
@@ -5242,7 +5239,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>1000</v>
       </c>
@@ -5253,7 +5250,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>1000</v>
       </c>
@@ -5264,7 +5261,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>1000</v>
       </c>
@@ -5275,7 +5272,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>1000</v>
       </c>
@@ -5286,7 +5283,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>1000</v>
       </c>
@@ -5297,7 +5294,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>1000</v>
       </c>
@@ -5308,7 +5305,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>1000</v>
       </c>
@@ -5319,7 +5316,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>1000</v>
       </c>
@@ -5330,7 +5327,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>1000</v>
       </c>
@@ -5341,7 +5338,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A49">
         <v>1000</v>
       </c>
@@ -5352,7 +5349,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A50">
         <v>1000</v>
       </c>
@@ -5363,7 +5360,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A51">
         <v>1000</v>
       </c>
@@ -5374,7 +5371,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A52">
         <v>1000</v>
       </c>
@@ -5385,7 +5382,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A53">
         <v>1000</v>
       </c>
@@ -5396,7 +5393,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A54">
         <v>1000</v>
       </c>
@@ -5407,7 +5404,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A55">
         <v>1000</v>
       </c>
@@ -5418,7 +5415,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A56">
         <v>1000</v>
       </c>
@@ -5429,7 +5426,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A57">
         <v>1000</v>
       </c>
@@ -5440,7 +5437,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A58">
         <v>1000</v>
       </c>
@@ -5451,7 +5448,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A59">
         <v>1000</v>
       </c>
@@ -5462,7 +5459,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A60">
         <v>1000</v>
       </c>
@@ -5473,7 +5470,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A61">
         <v>1000</v>
       </c>
@@ -5484,7 +5481,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A62">
         <v>1000</v>
       </c>
@@ -5495,7 +5492,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A63">
         <v>1000</v>
       </c>
@@ -5506,7 +5503,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A64">
         <v>1000</v>
       </c>
@@ -5517,7 +5514,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A65">
         <v>1000</v>
       </c>
@@ -5528,7 +5525,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A66">
         <v>1000</v>
       </c>
@@ -5539,7 +5536,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A67">
         <v>1000</v>
       </c>
@@ -5550,7 +5547,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A68">
         <v>1000</v>
       </c>
@@ -5561,7 +5558,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A69">
         <v>1000</v>
       </c>
@@ -5572,7 +5569,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A70">
         <v>1000</v>
       </c>
@@ -5583,7 +5580,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A71">
         <v>1000</v>
       </c>
@@ -5594,7 +5591,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A72">
         <v>1000</v>
       </c>
@@ -5605,7 +5602,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A73">
         <v>1000</v>
       </c>
@@ -5616,7 +5613,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A74">
         <v>1000</v>
       </c>
@@ -5627,7 +5624,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A75">
         <v>1000</v>
       </c>
@@ -5638,7 +5635,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A76">
         <v>1000</v>
       </c>
@@ -5649,7 +5646,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A77">
         <v>1000</v>
       </c>
@@ -5660,7 +5657,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A78">
         <v>1000</v>
       </c>
@@ -5671,7 +5668,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A79">
         <v>1000</v>
       </c>
@@ -5682,7 +5679,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="80" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A80">
         <v>1000</v>
       </c>
@@ -5693,7 +5690,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A81">
         <v>1000</v>
       </c>
@@ -5704,7 +5701,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="82" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A82">
         <v>1000</v>
       </c>
@@ -5715,7 +5712,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="83" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A83">
         <v>1000</v>
       </c>
@@ -5726,7 +5723,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="84" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A84">
         <v>1000</v>
       </c>
@@ -5737,7 +5734,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="85" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A85">
         <v>1000</v>
       </c>
@@ -5748,7 +5745,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="86" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A86">
         <v>1000</v>
       </c>
@@ -5759,7 +5756,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="87" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A87">
         <v>1000</v>
       </c>
@@ -5770,7 +5767,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="88" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A88">
         <v>1000</v>
       </c>
@@ -5781,7 +5778,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="89" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A89">
         <v>1000</v>
       </c>
@@ -5792,7 +5789,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="90" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A90">
         <v>1000</v>
       </c>
@@ -5803,7 +5800,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="91" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A91">
         <v>1000</v>
       </c>
@@ -5814,7 +5811,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="92" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A92">
         <v>1000</v>
       </c>
@@ -5825,7 +5822,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="93" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A93">
         <v>1000</v>
       </c>
@@ -5836,7 +5833,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="94" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A94">
         <v>1000</v>
       </c>
@@ -5847,7 +5844,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="95" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A95">
         <v>1000</v>
       </c>
@@ -5858,7 +5855,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="96" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A96">
         <v>1000</v>
       </c>
@@ -5869,7 +5866,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="97" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A97">
         <v>1000</v>
       </c>
@@ -5880,7 +5877,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="98" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A98">
         <v>1000</v>
       </c>
@@ -5891,7 +5888,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="99" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A99">
         <v>1000</v>
       </c>
@@ -5902,7 +5899,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="100" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A100">
         <v>1000</v>
       </c>
@@ -5913,7 +5910,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="101" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A101">
         <v>1000</v>
       </c>
@@ -5924,7 +5921,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="102" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A102">
         <v>1000</v>
       </c>
@@ -5935,7 +5932,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="103" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A103">
         <v>2000</v>
       </c>
@@ -5947,7 +5944,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="104" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A104">
         <v>2000</v>
       </c>
@@ -5959,7 +5956,7 @@
         <v>0.92797545119453517</v>
       </c>
     </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="105" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A105">
         <v>2000</v>
       </c>
@@ -5971,7 +5968,7 @@
         <v>0.86113843801970102</v>
       </c>
     </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="106" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A106">
         <v>2000</v>
       </c>
@@ -5983,7 +5980,7 @@
         <v>0.79911533056228934</v>
       </c>
     </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="107" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A107">
         <v>2000</v>
       </c>
@@ -5995,7 +5992,7 @@
         <v>0.74155940943501053</v>
       </c>
     </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="108" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A108">
         <v>2000</v>
       </c>
@@ -6007,7 +6004,7 @@
         <v>0.68814892755800683</v>
       </c>
     </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="109" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A109">
         <v>2000</v>
       </c>
@@ -6019,7 +6016,7 @@
         <v>0.6385853115396769</v>
       </c>
     </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="110" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A110">
         <v>2000</v>
       </c>
@@ -6031,7 +6028,7 @@
         <v>0.59259149260223443</v>
       </c>
     </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="111" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A111">
         <v>2000</v>
       </c>
@@ -6043,7 +6040,7 @@
         <v>0.54991035772160157</v>
       </c>
     </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="112" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A112">
         <v>2000</v>
       </c>
@@ -6055,7 +6052,7 @@
         <v>0.51030331232325143</v>
       </c>
     </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="113" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A113">
         <v>2000</v>
       </c>
@@ -6067,7 +6064,7 @@
         <v>0.47354894649923496</v>
       </c>
     </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="114" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A114">
         <v>2000</v>
       </c>
@@ -6079,7 +6076,7 @@
         <v>0.43944179729032434</v>
       </c>
     </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="115" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A115">
         <v>2000</v>
       </c>
@@ -6091,7 +6088,7 @@
         <v>0.4077912001142262</v>
       </c>
     </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="116" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A116">
         <v>2000</v>
       </c>
@@ -6103,7 +6100,7 @@
         <v>0.37842022291916005</v>
       </c>
     </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="117" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A117">
         <v>2000</v>
       </c>
@@ -6115,7 +6112,7 @@
         <v>0.35116467710454408</v>
       </c>
     </row>
-    <row r="118" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="118" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A118">
         <v>2000</v>
       </c>
@@ -6127,7 +6124,7 @@
         <v>0.32587219967967251</v>
       </c>
     </row>
-    <row r="119" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="119" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A119">
         <v>2000</v>
       </c>
@@ -6139,7 +6136,7 @@
         <v>0.30240140152949979</v>
       </c>
     </row>
-    <row r="120" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="120" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A120">
         <v>2000</v>
       </c>
@@ -6151,7 +6148,7 @@
         <v>0.28062107702619732</v>
       </c>
     </row>
-    <row r="121" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="121" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A121">
         <v>2000</v>
       </c>
@@ -6163,7 +6160,7 @@
         <v>0.26040947056808189</v>
       </c>
     </row>
-    <row r="122" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="122" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A122">
         <v>2000</v>
       </c>
@@ -6175,7 +6172,7 @@
         <v>0.24165359594574579</v>
       </c>
     </row>
-    <row r="123" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="123" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A123">
         <v>2000</v>
       </c>
@@ -6187,7 +6184,7 @@
         <v>0.22424860473053532</v>
       </c>
     </row>
-    <row r="124" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="124" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A124">
         <v>2000</v>
       </c>
@@ -6199,7 +6196,7 @@
         <v>0.20809720015456348</v>
       </c>
     </row>
-    <row r="125" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="125" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A125">
         <v>2000</v>
       </c>
@@ -6211,7 +6208,7 @@
         <v>0.19310909320575054</v>
       </c>
     </row>
-    <row r="126" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="126" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A126">
         <v>2000</v>
       </c>
@@ -6223,7 +6220,7 @@
         <v>0.17920049789737391</v>
       </c>
     </row>
-    <row r="127" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="127" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A127">
         <v>2000</v>
       </c>
@@ -6235,7 +6232,7 @@
         <v>0.16629366289060088</v>
       </c>
     </row>
-    <row r="128" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="128" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A128">
         <v>2000</v>
       </c>
@@ -6247,7 +6244,7 @@
         <v>0.15431643685169727</v>
       </c>
     </row>
-    <row r="129" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="129" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A129">
         <v>2000</v>
       </c>
@@ -6259,7 +6256,7 @@
         <v>0.14320186511418675</v>
       </c>
     </row>
-    <row r="130" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="130" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A130">
         <v>2000</v>
       </c>
@@ -6271,7 +6268,7 @@
         <v>0.13288781539123642</v>
       </c>
     </row>
-    <row r="131" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="131" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A131">
         <v>2000</v>
       </c>
@@ -6283,7 +6280,7 @@
         <v>0.12331663044593871</v>
       </c>
     </row>
-    <row r="132" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="132" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A132">
         <v>2000</v>
       </c>
@@ -6295,7 +6292,7 @@
         <v>0.11443480577785975</v>
       </c>
     </row>
-    <row r="133" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="133" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A133">
         <v>2000</v>
       </c>
@@ -6307,7 +6304,7 @@
         <v>0.10619269052406835</v>
       </c>
     </row>
-    <row r="134" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="134" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A134">
         <v>2000</v>
       </c>
@@ -6319,7 +6316,7 @@
         <v>9.8544209902633975E-2</v>
       </c>
     </row>
-    <row r="135" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="135" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A135">
         <v>2000</v>
       </c>
@@ -6331,7 +6328,7 @@
         <v>9.1446607647005754E-2</v>
       </c>
     </row>
-    <row r="136" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="136" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A136">
         <v>2000</v>
       </c>
@@ -6343,7 +6340,7 @@
         <v>8.4860206991439771E-2</v>
       </c>
     </row>
-    <row r="137" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="137" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A137">
         <v>2000</v>
       </c>
@@ -6355,7 +6352,7 @@
         <v>7.8748188871342967E-2</v>
       </c>
     </row>
-    <row r="138" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="138" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A138">
         <v>2000</v>
       </c>
@@ -6367,7 +6364,7 @@
         <v>7.3076386098636967E-2</v>
       </c>
     </row>
-    <row r="139" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="139" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A139">
         <v>2000</v>
       </c>
@@ -6379,7 +6376,7 @@
         <v>6.7813092361548713E-2</v>
       </c>
     </row>
-    <row r="140" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="140" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A140">
         <v>2000</v>
       </c>
@@ -6391,7 +6388,7 @@
         <v>6.2928884981104827E-2</v>
       </c>
     </row>
-    <row r="141" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="141" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A141">
         <v>2000</v>
       </c>
@@ -6403,7 +6400,7 @@
         <v>5.8396460433509767E-2</v>
       </c>
     </row>
-    <row r="142" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="142" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A142">
         <v>2000</v>
       </c>
@@ -6415,7 +6412,7 @@
         <v>5.4190481718950051E-2</v>
       </c>
     </row>
-    <row r="143" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="143" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A143">
         <v>2000</v>
       </c>
@@ -6427,7 +6424,7 @@
         <v>5.0287436723591865E-2</v>
       </c>
     </row>
-    <row r="144" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="144" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A144">
         <v>2000</v>
       </c>
@@ -6438,7 +6435,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="145" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="145" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A145">
         <v>2000</v>
       </c>
@@ -6449,7 +6446,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="146" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="146" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A146">
         <v>2000</v>
       </c>
@@ -6460,7 +6457,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="147" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="147" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A147">
         <v>2000</v>
       </c>
@@ -6471,7 +6468,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="148" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="148" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A148">
         <v>2000</v>
       </c>
@@ -6482,7 +6479,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="149" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="149" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A149">
         <v>2000</v>
       </c>
@@ -6493,7 +6490,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="150" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="150" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A150">
         <v>2000</v>
       </c>
@@ -6504,7 +6501,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="151" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="151" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A151">
         <v>2000</v>
       </c>
@@ -6515,7 +6512,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="152" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="152" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A152">
         <v>2000</v>
       </c>
@@ -6526,7 +6523,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="153" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="153" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A153">
         <v>2000</v>
       </c>
@@ -6537,7 +6534,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="154" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="154" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A154">
         <v>2000</v>
       </c>
@@ -6548,7 +6545,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="155" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="155" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A155">
         <v>2000</v>
       </c>
@@ -6559,7 +6556,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="156" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="156" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A156">
         <v>2000</v>
       </c>
@@ -6570,7 +6567,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="157" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="157" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A157">
         <v>2000</v>
       </c>
@@ -6581,7 +6578,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="158" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="158" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A158">
         <v>2000</v>
       </c>
@@ -6592,7 +6589,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="159" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="159" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A159">
         <v>2000</v>
       </c>
@@ -6603,7 +6600,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="160" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="160" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A160">
         <v>2000</v>
       </c>
@@ -6614,7 +6611,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="161" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="161" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A161">
         <v>2000</v>
       </c>
@@ -6625,7 +6622,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="162" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="162" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A162">
         <v>2000</v>
       </c>
@@ -6636,7 +6633,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="163" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="163" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A163">
         <v>2000</v>
       </c>
@@ -6647,7 +6644,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="164" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="164" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A164">
         <v>2000</v>
       </c>
@@ -6658,7 +6655,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="165" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="165" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A165">
         <v>2000</v>
       </c>
@@ -6669,7 +6666,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="166" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="166" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A166">
         <v>2000</v>
       </c>
@@ -6680,7 +6677,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="167" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="167" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A167">
         <v>2000</v>
       </c>
@@ -6691,7 +6688,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="168" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="168" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A168">
         <v>2000</v>
       </c>
@@ -6702,7 +6699,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="169" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="169" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A169">
         <v>2000</v>
       </c>
@@ -6713,7 +6710,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="170" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="170" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A170">
         <v>2000</v>
       </c>
@@ -6724,7 +6721,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="171" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="171" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A171">
         <v>2000</v>
       </c>
@@ -6735,7 +6732,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="172" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="172" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A172">
         <v>2000</v>
       </c>
@@ -6746,7 +6743,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="173" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="173" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A173">
         <v>2000</v>
       </c>
@@ -6757,7 +6754,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="174" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="174" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A174">
         <v>2000</v>
       </c>
@@ -6768,7 +6765,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="175" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="175" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A175">
         <v>2000</v>
       </c>
@@ -6779,7 +6776,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="176" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="176" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A176">
         <v>2000</v>
       </c>
@@ -6790,7 +6787,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="177" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="177" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A177">
         <v>2000</v>
       </c>
@@ -6801,7 +6798,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="178" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="178" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A178">
         <v>2000</v>
       </c>
@@ -6812,7 +6809,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="179" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="179" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A179">
         <v>2000</v>
       </c>
@@ -6823,7 +6820,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="180" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="180" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A180">
         <v>2000</v>
       </c>
@@ -6834,7 +6831,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="181" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="181" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A181">
         <v>2000</v>
       </c>
@@ -6845,7 +6842,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="182" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="182" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A182">
         <v>2000</v>
       </c>
@@ -6856,7 +6853,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="183" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="183" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A183">
         <v>2000</v>
       </c>
@@ -6867,7 +6864,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="184" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="184" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A184">
         <v>2000</v>
       </c>
@@ -6878,7 +6875,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="185" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="185" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A185">
         <v>2000</v>
       </c>
@@ -6889,7 +6886,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="186" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="186" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A186">
         <v>2000</v>
       </c>
@@ -6900,7 +6897,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="187" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="187" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A187">
         <v>2000</v>
       </c>
@@ -6911,7 +6908,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="188" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="188" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A188">
         <v>2000</v>
       </c>
@@ -6922,7 +6919,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="189" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="189" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A189">
         <v>2000</v>
       </c>
@@ -6933,7 +6930,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="190" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="190" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A190">
         <v>2000</v>
       </c>
@@ -6944,7 +6941,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="191" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="191" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A191">
         <v>2000</v>
       </c>
@@ -6955,7 +6952,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="192" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="192" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A192">
         <v>2000</v>
       </c>
@@ -6966,7 +6963,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="193" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="193" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A193">
         <v>2000</v>
       </c>
@@ -6977,7 +6974,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="194" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="194" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A194">
         <v>2000</v>
       </c>
@@ -6988,7 +6985,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="195" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="195" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A195">
         <v>2000</v>
       </c>
@@ -6999,7 +6996,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="196" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="196" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A196">
         <v>2000</v>
       </c>
@@ -7010,7 +7007,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="197" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="197" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A197">
         <v>2000</v>
       </c>
@@ -7021,7 +7018,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="198" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="198" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A198">
         <v>2000</v>
       </c>
@@ -7032,7 +7029,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="199" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="199" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A199">
         <v>2000</v>
       </c>
@@ -7043,7 +7040,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="200" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="200" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A200">
         <v>2000</v>
       </c>
@@ -7054,7 +7051,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="201" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="201" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A201">
         <v>2000</v>
       </c>
@@ -7065,7 +7062,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="202" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="202" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A202">
         <v>2000</v>
       </c>
@@ -7076,7 +7073,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="203" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="203" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A203">
         <v>2000</v>
       </c>
@@ -7087,7 +7084,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="204" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="204" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A204">
         <v>3000</v>
       </c>
@@ -7099,7 +7096,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="205" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="205" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A205">
         <v>3000</v>
       </c>
@@ -7111,7 +7108,7 @@
         <v>0.9513879759503846</v>
       </c>
     </row>
-    <row r="206" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="206" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A206">
         <v>3000</v>
       </c>
@@ -7123,7 +7120,7 @@
         <v>0.90513908078296956</v>
       </c>
     </row>
-    <row r="207" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="207" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A207">
         <v>3000</v>
       </c>
@@ -7135,7 +7132,7 @@
         <v>0.86113843801970102</v>
       </c>
     </row>
-    <row r="208" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="208" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A208">
         <v>3000</v>
       </c>
@@ -7147,7 +7144,7 @@
         <v>0.81927675556063906</v>
       </c>
     </row>
-    <row r="209" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="209" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A209">
         <v>3000</v>
       </c>
@@ -7159,7 +7156,7 @@
         <v>0.77945005421603442</v>
       </c>
     </row>
-    <row r="210" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="210" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A210">
         <v>3000</v>
       </c>
@@ -7171,7 +7168,7 @@
         <v>0.74155940943501042</v>
       </c>
     </row>
-    <row r="211" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="211" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A211">
         <v>3000</v>
       </c>
@@ -7183,7 +7180,7 @@
         <v>0.70551070558933715</v>
       </c>
     </row>
-    <row r="212" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="212" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A212">
         <v>3000</v>
       </c>
@@ -7195,7 +7192,7 @@
         <v>0.67121440220196715</v>
       </c>
     </row>
-    <row r="213" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="213" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A213">
         <v>3000</v>
       </c>
@@ -7207,7 +7204,7 @@
         <v>0.6385853115396769</v>
       </c>
     </row>
-    <row r="214" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="214" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A214">
         <v>3000</v>
       </c>
@@ -7219,7 +7216,7 @@
         <v>0.60754238701737895</v>
       </c>
     </row>
-    <row r="215" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="215" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A215">
         <v>3000</v>
       </c>
@@ -7231,7 +7228,7 @@
         <v>0.57800852188852936</v>
       </c>
     </row>
-    <row r="216" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="216" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A216">
         <v>3000</v>
       </c>
@@ -7243,7 +7240,7 @@
         <v>0.54991035772160146</v>
       </c>
     </row>
-    <row r="217" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="217" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A217">
         <v>3000</v>
       </c>
@@ -7255,7 +7252,7 @@
         <v>0.52317810218690641</v>
       </c>
     </row>
-    <row r="218" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="218" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A218">
         <v>3000</v>
       </c>
@@ -7267,7 +7264,7 @@
         <v>0.49774535570116435</v>
       </c>
     </row>
-    <row r="219" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="219" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A219">
         <v>3000</v>
       </c>
@@ -7279,7 +7276,7 @@
         <v>0.47354894649923496</v>
       </c>
     </row>
-    <row r="220" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="220" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A220">
         <v>3000</v>
       </c>
@@ -7291,7 +7288,7 @@
         <v>0.4505287737233441</v>
       </c>
     </row>
-    <row r="221" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="221" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A221">
         <v>3000</v>
       </c>
@@ -7303,7 +7300,7 @@
         <v>0.42862765814006115</v>
       </c>
     </row>
-    <row r="222" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="222" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A222">
         <v>3000</v>
       </c>
@@ -7315,7 +7312,7 @@
         <v>0.40779120011422615</v>
       </c>
     </row>
-    <row r="223" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="223" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A223">
         <v>3000</v>
       </c>
@@ -7327,7 +7324,7 @@
         <v>0.3879676444870519</v>
       </c>
     </row>
-    <row r="224" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="224" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A224">
         <v>3000</v>
       </c>
@@ -7339,7 +7336,7 @@
         <v>0.36910775202277468</v>
       </c>
     </row>
-    <row r="225" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="225" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A225">
         <v>3000</v>
       </c>
@@ -7351,7 +7348,7 @@
         <v>0.35116467710454408</v>
       </c>
     </row>
-    <row r="226" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="226" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A226">
         <v>3000</v>
       </c>
@@ -7363,7 +7360,7 @@
         <v>0.33409385137576253</v>
       </c>
     </row>
-    <row r="227" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="227" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A227">
         <v>3000</v>
       </c>
@@ -7375,7 +7372,7 @@
         <v>0.31785287303785531</v>
       </c>
     </row>
-    <row r="228" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="228" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A228">
         <v>3000</v>
       </c>
@@ -7387,7 +7384,7 @@
         <v>0.30240140152949974</v>
       </c>
     </row>
-    <row r="229" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="229" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A229">
         <v>3000</v>
       </c>
@@ -7399,7 +7396,7 @@
         <v>0.28770105732571033</v>
       </c>
     </row>
-    <row r="230" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="230" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A230">
         <v>3000</v>
       </c>
@@ -7411,7 +7408,7 @@
         <v>0.27371532660789311</v>
       </c>
     </row>
-    <row r="231" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="231" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A231">
         <v>3000</v>
       </c>
@@ -7423,7 +7420,7 @@
         <v>0.26040947056808184</v>
       </c>
     </row>
-    <row r="232" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="232" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A232">
         <v>3000</v>
       </c>
@@ -7435,7 +7432,7 @@
         <v>0.24775043912207861</v>
       </c>
     </row>
-    <row r="233" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="233" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A233">
         <v>3000</v>
       </c>
@@ -7447,7 +7444,7 @@
         <v>0.23570678881717338</v>
       </c>
     </row>
-    <row r="234" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="234" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A234">
         <v>3000</v>
       </c>
@@ -7459,7 +7456,7 @@
         <v>0.22424860473053532</v>
       </c>
     </row>
-    <row r="235" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="235" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A235">
         <v>3000</v>
       </c>
@@ -7471,7 +7468,7 @@
         <v>0.21334742616428182</v>
       </c>
     </row>
-    <row r="236" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="236" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A236">
         <v>3000</v>
       </c>
@@ -7483,7 +7480,7 @@
         <v>0.20297617595266018</v>
       </c>
     </row>
-    <row r="237" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="237" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A237">
         <v>3000</v>
       </c>
@@ -7495,7 +7492,7 @@
         <v>0.19310909320575054</v>
       </c>
     </row>
-    <row r="238" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="238" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A238">
         <v>3000</v>
       </c>
@@ -7507,7 +7504,7 @@
         <v>0.18372166932263315</v>
       </c>
     </row>
-    <row r="239" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="239" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A239">
         <v>3000</v>
       </c>
@@ -7519,7 +7516,7 @@
         <v>0.1747905871150858</v>
       </c>
     </row>
-    <row r="240" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="240" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A240">
         <v>3000</v>
       </c>
@@ -7531,7 +7528,7 @@
         <v>0.16629366289060085</v>
       </c>
     </row>
-    <row r="241" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="241" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A241">
         <v>3000</v>
       </c>
@@ -7543,7 +7540,7 @@
         <v>0.15820979135086433</v>
       </c>
     </row>
-    <row r="242" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="242" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A242">
         <v>3000</v>
       </c>
@@ -7555,7 +7552,7 @@
         <v>0.15051889316883146</v>
       </c>
     </row>
-    <row r="243" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="243" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A243">
         <v>3000</v>
       </c>
@@ -7567,7 +7564,7 @@
         <v>0.14320186511418673</v>
       </c>
     </row>
-    <row r="244" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="244" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A244">
         <v>3000</v>
       </c>
@@ -7579,7 +7576,7 @@
         <v>0.13624053260330612</v>
       </c>
     </row>
-    <row r="245" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="245" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A245">
         <v>3000</v>
       </c>
@@ -7591,7 +7588,7 @@
         <v>0.12961760455586177</v>
       </c>
     </row>
-    <row r="246" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="246" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A246">
         <v>3000</v>
       </c>
@@ -7603,7 +7600,7 @@
         <v>0.12331663044593871</v>
       </c>
     </row>
-    <row r="247" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="247" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A247">
         <v>3000</v>
       </c>
@@ -7615,7 +7612,7 @@
         <v>0.1173219594409832</v>
       </c>
     </row>
-    <row r="248" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="248" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A248">
         <v>3000</v>
       </c>
@@ -7627,7 +7624,7 @@
         <v>0.11161870152709011</v>
       </c>
     </row>
-    <row r="249" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="249" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A249">
         <v>3000</v>
       </c>
@@ -7639,7 +7636,7 @@
         <v>0.10619269052406835</v>
       </c>
     </row>
-    <row r="250" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="250" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A250">
         <v>3000</v>
       </c>
@@ -7651,7 +7648,7 @@
         <v>0.10103044889841897</v>
       </c>
     </row>
-    <row r="251" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="251" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A251">
         <v>3000</v>
       </c>
@@ -7663,7 +7660,7 @@
         <v>9.6119154286825575E-2</v>
       </c>
     </row>
-    <row r="252" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="252" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A252">
         <v>3000</v>
       </c>
@@ -7675,7 +7672,7 @@
         <v>9.1446607647005712E-2</v>
       </c>
     </row>
-    <row r="253" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="253" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A253">
         <v>3000</v>
       </c>
@@ -7687,7 +7684,7 @@
         <v>8.7001202956813725E-2</v>
       </c>
     </row>
-    <row r="254" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="254" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A254">
         <v>3000</v>
       </c>
@@ -7699,7 +7696,7 @@
         <v>8.2771898386331658E-2</v>
       </c>
     </row>
-    <row r="255" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="255" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A255">
         <v>3000</v>
       </c>
@@ -7711,7 +7708,7 @@
         <v>7.8748188871342967E-2</v>
       </c>
     </row>
-    <row r="256" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="256" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A256">
         <v>3000</v>
       </c>
@@ -7723,7 +7720,7 @@
         <v>7.4920080020065588E-2</v>
       </c>
     </row>
-    <row r="257" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="257" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A257">
         <v>3000</v>
       </c>
@@ -7735,7 +7732,7 @@
         <v>7.1278063288331042E-2</v>
       </c>
     </row>
-    <row r="258" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="258" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A258">
         <v>3000</v>
       </c>
@@ -7747,7 +7744,7 @@
         <v>6.7813092361548685E-2</v>
       </c>
     </row>
-    <row r="259" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="259" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A259">
         <v>3000</v>
       </c>
@@ -7759,7 +7756,7 @@
         <v>6.4516560684790281E-2</v>
       </c>
     </row>
-    <row r="260" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="260" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A260">
         <v>3000</v>
       </c>
@@ -7771,7 +7768,7 @@
         <v>6.138028008518278E-2</v>
       </c>
     </row>
-    <row r="261" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="261" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A261">
         <v>3000</v>
       </c>
@@ -7783,7 +7780,7 @@
         <v>5.8396460433509767E-2</v>
       </c>
     </row>
-    <row r="262" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="262" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A262">
         <v>3000</v>
       </c>
@@ -7795,7 +7792,7 @@
         <v>5.5557690294503567E-2</v>
       </c>
     </row>
-    <row r="263" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="263" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A263">
         <v>3000</v>
       </c>
@@ -7807,7 +7804,7 @@
         <v>5.2856918517766076E-2</v>
       </c>
     </row>
-    <row r="264" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="264" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A264">
         <v>3000</v>
       </c>
@@ -7819,7 +7816,7 @@
         <v>5.0287436723591865E-2</v>
       </c>
     </row>
-    <row r="265" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="265" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A265">
         <v>3000</v>
       </c>
@@ -7830,7 +7827,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="266" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="266" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A266">
         <v>3000</v>
       </c>
@@ -7841,7 +7838,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="267" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="267" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A267">
         <v>3000</v>
       </c>
@@ -7852,7 +7849,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="268" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="268" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A268">
         <v>3000</v>
       </c>
@@ -7863,7 +7860,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="269" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="269" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A269">
         <v>3000</v>
       </c>
@@ -7874,7 +7871,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="270" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="270" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A270">
         <v>3000</v>
       </c>
@@ -7885,7 +7882,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="271" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="271" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A271">
         <v>3000</v>
       </c>
@@ -7896,7 +7893,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="272" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="272" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A272">
         <v>3000</v>
       </c>
@@ -7907,7 +7904,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="273" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="273" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A273">
         <v>3000</v>
       </c>
@@ -7918,7 +7915,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="274" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="274" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A274">
         <v>3000</v>
       </c>
@@ -7929,7 +7926,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="275" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="275" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A275">
         <v>3000</v>
       </c>
@@ -7940,7 +7937,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="276" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="276" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A276">
         <v>3000</v>
       </c>
@@ -7951,7 +7948,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="277" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="277" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A277">
         <v>3000</v>
       </c>
@@ -7962,7 +7959,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="278" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="278" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A278">
         <v>3000</v>
       </c>
@@ -7973,7 +7970,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="279" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="279" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A279">
         <v>3000</v>
       </c>
@@ -7984,7 +7981,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="280" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="280" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A280">
         <v>3000</v>
       </c>
@@ -7995,7 +7992,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="281" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="281" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A281">
         <v>3000</v>
       </c>
@@ -8006,7 +8003,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="282" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="282" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A282">
         <v>3000</v>
       </c>
@@ -8017,7 +8014,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="283" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="283" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A283">
         <v>3000</v>
       </c>
@@ -8028,7 +8025,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="284" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="284" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A284">
         <v>3000</v>
       </c>
@@ -8039,7 +8036,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="285" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="285" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A285">
         <v>3000</v>
       </c>
@@ -8050,7 +8047,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="286" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="286" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A286">
         <v>3000</v>
       </c>
@@ -8061,7 +8058,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="287" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="287" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A287">
         <v>3000</v>
       </c>
@@ -8072,7 +8069,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="288" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="288" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A288">
         <v>3000</v>
       </c>
@@ -8083,7 +8080,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="289" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="289" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A289">
         <v>3000</v>
       </c>
@@ -8094,7 +8091,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="290" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="290" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A290">
         <v>3000</v>
       </c>
@@ -8105,7 +8102,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="291" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="291" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A291">
         <v>3000</v>
       </c>
@@ -8116,7 +8113,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="292" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="292" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A292">
         <v>3000</v>
       </c>
@@ -8127,7 +8124,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="293" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="293" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A293">
         <v>3000</v>
       </c>
@@ -8138,7 +8135,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="294" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="294" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A294">
         <v>3000</v>
       </c>
@@ -8149,7 +8146,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="295" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="295" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A295">
         <v>3000</v>
       </c>
@@ -8160,7 +8157,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="296" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="296" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A296">
         <v>3000</v>
       </c>
@@ -8171,7 +8168,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="297" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="297" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A297">
         <v>3000</v>
       </c>
@@ -8182,7 +8179,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="298" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="298" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A298">
         <v>3000</v>
       </c>
@@ -8193,7 +8190,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="299" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="299" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A299">
         <v>3000</v>
       </c>
@@ -8204,7 +8201,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="300" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="300" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A300">
         <v>3000</v>
       </c>
@@ -8215,7 +8212,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="301" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="301" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A301">
         <v>3000</v>
       </c>
@@ -8226,7 +8223,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="302" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="302" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A302">
         <v>3000</v>
       </c>
@@ -8237,7 +8234,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="303" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="303" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A303">
         <v>3000</v>
       </c>
@@ -8248,7 +8245,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="304" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="304" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A304">
         <v>3000</v>
       </c>
@@ -8259,7 +8256,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="305" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="305" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A305">
         <v>4000</v>
       </c>
@@ -8271,7 +8268,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="306" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="306" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A306">
         <v>4000</v>
       </c>
@@ -8283,7 +8280,7 @@
         <v>0.96331482454830686</v>
       </c>
     </row>
-    <row r="307" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="307" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A307">
         <v>4000</v>
       </c>
@@ -8295,7 +8292,7 @@
         <v>0.92797545119453517</v>
       </c>
     </row>
-    <row r="308" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="308" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A308">
         <v>4000</v>
       </c>
@@ -8307,7 +8304,7 @@
         <v>0.89393250895259946</v>
       </c>
     </row>
-    <row r="309" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="309" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A309">
         <v>4000</v>
       </c>
@@ -8319,7 +8316,7 @@
         <v>0.86113843801970102</v>
       </c>
     </row>
-    <row r="310" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="310" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A310">
         <v>4000</v>
       </c>
@@ -8331,7 +8328,7 @@
         <v>0.82954742333275133</v>
       </c>
     </row>
-    <row r="311" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="311" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A311">
         <v>4000</v>
       </c>
@@ -8343,7 +8340,7 @@
         <v>0.79911533056228934</v>
       </c>
     </row>
-    <row r="312" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="312" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A312">
         <v>4000</v>
       </c>
@@ -8355,7 +8352,7 @@
         <v>0.76979964445447391</v>
       </c>
     </row>
-    <row r="313" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="313" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A313">
         <v>4000</v>
       </c>
@@ -8367,7 +8364,7 @@
         <v>0.74155940943501053</v>
       </c>
     </row>
-    <row r="314" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="314" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A314">
         <v>4000</v>
       </c>
@@ -8379,7 +8376,7 @@
         <v>0.71435517239203317</v>
       </c>
     </row>
-    <row r="315" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="315" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A315">
         <v>4000</v>
       </c>
@@ -8391,7 +8388,7 @@
         <v>0.68814892755800683</v>
       </c>
     </row>
-    <row r="316" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="316" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A316">
         <v>4000</v>
       </c>
@@ -8403,7 +8400,7 @@
         <v>0.66290406341364683</v>
       </c>
     </row>
-    <row r="317" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="317" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A317">
         <v>4000</v>
       </c>
@@ -8415,7 +8412,7 @@
         <v>0.6385853115396769</v>
       </c>
     </row>
-    <row r="318" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="318" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A318">
         <v>4000</v>
       </c>
@@ -8427,7 +8424,7 @@
         <v>0.61515869734496975</v>
       </c>
     </row>
-    <row r="319" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="319" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A319">
         <v>4000</v>
       </c>
@@ -8439,7 +8436,7 @@
         <v>0.59259149260223443</v>
       </c>
     </row>
-    <row r="320" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="320" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A320">
         <v>4000</v>
       </c>
@@ -8451,7 +8448,7 @@
         <v>0.57085216972494068</v>
       </c>
     </row>
-    <row r="321" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="321" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A321">
         <v>4000</v>
       </c>
@@ -8463,7 +8460,7 @@
         <v>0.54991035772160157</v>
       </c>
     </row>
-    <row r="322" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="322" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A322">
         <v>4000</v>
       </c>
@@ -8475,7 +8472,7 @@
         <v>0.52973679976588117</v>
       </c>
     </row>
-    <row r="323" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="323" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A323">
         <v>4000</v>
       </c>
@@ -8487,7 +8484,7 @@
         <v>0.51030331232325143</v>
       </c>
     </row>
-    <row r="324" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="324" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A324">
         <v>4000</v>
       </c>
@@ -8499,7 +8496,7 @@
         <v>0.49158274577709271</v>
       </c>
     </row>
-    <row r="325" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="325" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A325">
         <v>4000</v>
       </c>
@@ -8511,7 +8508,7 @@
         <v>0.47354894649923496</v>
       </c>
     </row>
-    <row r="326" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="326" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A326">
         <v>4000</v>
       </c>
@@ -8523,7 +8520,7 @@
         <v>0.45617672031194612</v>
       </c>
     </row>
-    <row r="327" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="327" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A327">
         <v>4000</v>
       </c>
@@ -8535,7 +8532,7 @@
         <v>0.43944179729032434</v>
       </c>
     </row>
-    <row r="328" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="328" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A328">
         <v>4000</v>
       </c>
@@ -8547,7 +8544,7 @@
         <v>0.42332079785592147</v>
       </c>
     </row>
-    <row r="329" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="329" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A329">
         <v>4000</v>
       </c>
@@ -8559,7 +8556,7 @@
         <v>0.4077912001142262</v>
       </c>
     </row>
-    <row r="330" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="330" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A330">
         <v>4000</v>
       </c>
@@ -8571,7 +8568,7 @@
         <v>0.39283130839037927</v>
       </c>
     </row>
-    <row r="331" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="331" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A331">
         <v>4000</v>
       </c>
@@ -8583,7 +8580,7 @@
         <v>0.37842022291916005</v>
       </c>
     </row>
-    <row r="332" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="332" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A332">
         <v>4000</v>
       </c>
@@ -8595,7 +8592,7 @@
         <v>0.36453781064690177</v>
       </c>
     </row>
-    <row r="333" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="333" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A333">
         <v>4000</v>
       </c>
@@ -8607,7 +8604,7 @@
         <v>0.35116467710454408</v>
       </c>
     </row>
-    <row r="334" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="334" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A334">
         <v>4000</v>
       </c>
@@ -8619,7 +8616,7 @@
         <v>0.33828213931252671</v>
       </c>
     </row>
-    <row r="335" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="335" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A335">
         <v>4000</v>
       </c>
@@ -8631,7 +8628,7 @@
         <v>0.32587219967967251</v>
       </c>
     </row>
-    <row r="336" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="336" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A336">
         <v>4000</v>
       </c>
@@ -8643,7 +8640,7 @@
         <v>0.31391752085959457</v>
       </c>
     </row>
-    <row r="337" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="337" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A337">
         <v>4000</v>
       </c>
@@ -8655,7 +8652,7 @@
         <v>0.30240140152949979</v>
       </c>
     </row>
-    <row r="338" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="338" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A338">
         <v>4000</v>
       </c>
@@ -8667,7 +8664,7 @@
         <v>0.29130775305755213</v>
       </c>
     </row>
-    <row r="339" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="339" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A339">
         <v>4000</v>
       </c>
@@ -8679,7 +8676,7 @@
         <v>0.28062107702619732</v>
       </c>
     </row>
-    <row r="340" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="340" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A340">
         <v>4000</v>
       </c>
@@ -8691,7 +8688,7 @@
         <v>0.2703264435800482</v>
       </c>
     </row>
-    <row r="341" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="341" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A341">
         <v>4000</v>
       </c>
@@ -8703,7 +8700,7 @@
         <v>0.26040947056808189</v>
       </c>
     </row>
-    <row r="342" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="342" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A342">
         <v>4000</v>
       </c>
@@ -8715,7 +8712,7 @@
         <v>0.25085630345100923</v>
       </c>
     </row>
-    <row r="343" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="343" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A343">
         <v>4000</v>
       </c>
@@ -8727,7 +8724,7 @@
         <v>0.24165359594574579</v>
       </c>
     </row>
-    <row r="344" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="344" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A344">
         <v>4000</v>
       </c>
@@ -8739,7 +8736,7 @@
         <v>0.23278849137994354</v>
       </c>
     </row>
-    <row r="345" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="345" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A345">
         <v>4000</v>
       </c>
@@ -8751,7 +8748,7 @@
         <v>0.22424860473053532</v>
       </c>
     </row>
-    <row r="346" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="346" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A346">
         <v>4000</v>
       </c>
@@ -8763,7 +8760,7 @@
         <v>0.21602200532119825</v>
       </c>
     </row>
-    <row r="347" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="347" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A347">
         <v>4000</v>
       </c>
@@ -8775,7 +8772,7 @@
         <v>0.20809720015456348</v>
       </c>
     </row>
-    <row r="348" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="348" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A348">
         <v>4000</v>
       </c>
@@ -8787,7 +8784,7 @@
         <v>0.20046311785588722</v>
       </c>
     </row>
-    <row r="349" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="349" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A349">
         <v>4000</v>
       </c>
@@ -8799,7 +8796,7 @@
         <v>0.19310909320575054</v>
       </c>
     </row>
-    <row r="350" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="350" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A350">
         <v>4000</v>
       </c>
@@ -8811,7 +8808,7 @@
         <v>0.1860248522401802</v>
       </c>
     </row>
-    <row r="351" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="351" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A351">
         <v>4000</v>
       </c>
@@ -8823,7 +8820,7 @@
         <v>0.17920049789737391</v>
       </c>
     </row>
-    <row r="352" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="352" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A352">
         <v>4000</v>
       </c>
@@ -8835,7 +8832,7 @@
         <v>0.17262649619097795</v>
       </c>
     </row>
-    <row r="353" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="353" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A353">
         <v>4000</v>
       </c>
@@ -8847,7 +8844,7 @@
         <v>0.16629366289060088</v>
       </c>
     </row>
-    <row r="354" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="354" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A354">
         <v>4000</v>
       </c>
@@ -8859,7 +8856,7 @@
         <v>0.16019315069095447</v>
       </c>
     </row>
-    <row r="355" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="355" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A355">
         <v>4000</v>
       </c>
@@ -8871,7 +8868,7 @@
         <v>0.15431643685169727</v>
       </c>
     </row>
-    <row r="356" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="356" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A356">
         <v>4000</v>
       </c>
@@ -8883,7 +8880,7 @@
         <v>0.14865531129071263</v>
       </c>
     </row>
-    <row r="357" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="357" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A357">
         <v>4000</v>
       </c>
@@ -8895,7 +8892,7 @@
         <v>0.14320186511418675</v>
       </c>
     </row>
-    <row r="358" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="358" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A358">
         <v>4000</v>
       </c>
@@ -8907,7 +8904,7 @@
         <v>0.13794847956746314</v>
       </c>
     </row>
-    <row r="359" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="359" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A359">
         <v>4000</v>
       </c>
@@ -8919,7 +8916,7 @@
         <v>0.13288781539123642</v>
       </c>
     </row>
-    <row r="360" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="360" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A360">
         <v>4000</v>
       </c>
@@ -8931,7 +8928,7 @@
         <v>0.1280128025682167</v>
       </c>
     </row>
-    <row r="361" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="361" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A361">
         <v>4000</v>
       </c>
@@ -8943,7 +8940,7 @@
         <v>0.12331663044593871</v>
       </c>
     </row>
-    <row r="362" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="362" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A362">
         <v>4000</v>
       </c>
@@ -8955,7 +8952,7 @@
         <v>0.11879273822191785</v>
       </c>
     </row>
-    <row r="363" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="363" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A363">
         <v>4000</v>
       </c>
@@ -8967,7 +8964,7 @@
         <v>0.11443480577785975</v>
       </c>
     </row>
-    <row r="364" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="364" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A364">
         <v>4000</v>
       </c>
@@ -8979,7 +8976,7 @@
         <v>0.11023674485011849</v>
       </c>
     </row>
-    <row r="365" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="365" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A365">
         <v>4000</v>
       </c>
@@ -8991,7 +8988,7 @@
         <v>0.10619269052406835</v>
       </c>
     </row>
-    <row r="366" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="366" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A366">
         <v>4000</v>
       </c>
@@ -9003,7 +9000,7 @@
         <v>0.10229699304050556</v>
       </c>
     </row>
-    <row r="367" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="367" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A367">
         <v>4000</v>
       </c>
@@ -9015,7 +9012,7 @@
         <v>9.8544209902633975E-2</v>
       </c>
     </row>
-    <row r="368" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="368" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A368">
         <v>4000</v>
       </c>
@@ -9027,7 +9024,7 @@
         <v>9.4929098272607371E-2</v>
       </c>
     </row>
-    <row r="369" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="369" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A369">
         <v>4000</v>
       </c>
@@ -9039,7 +9036,7 @@
         <v>9.1446607647005754E-2</v>
       </c>
     </row>
-    <row r="370" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="370" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A370">
         <v>4000</v>
       </c>
@@ -9051,7 +9048,7 @@
         <v>8.8091872801013202E-2</v>
       </c>
     </row>
-    <row r="371" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="371" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A371">
         <v>4000</v>
       </c>
@@ -9063,7 +9060,7 @@
         <v>8.4860206991439771E-2</v>
       </c>
     </row>
-    <row r="372" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="372" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A372">
         <v>4000</v>
       </c>
@@ -9075,7 +9072,7 @@
         <v>8.1747095409091808E-2</v>
       </c>
     </row>
-    <row r="373" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="373" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A373">
         <v>4000</v>
       </c>
@@ -9087,7 +9084,7 @@
         <v>7.8748188871342967E-2</v>
       </c>
     </row>
-    <row r="374" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="374" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A374">
         <v>4000</v>
       </c>
@@ -9099,7 +9096,7 @@
         <v>7.5859297746094692E-2</v>
       </c>
     </row>
-    <row r="375" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="375" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A375">
         <v>4000</v>
       </c>
@@ -9111,7 +9108,7 @@
         <v>7.3076386098636967E-2</v>
       </c>
     </row>
-    <row r="376" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="376" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A376">
         <v>4000</v>
       </c>
@@ -9123,7 +9120,7 @@
         <v>7.0395566053232814E-2</v>
       </c>
     </row>
-    <row r="377" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="377" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A377">
         <v>4000</v>
       </c>
@@ -9135,7 +9132,7 @@
         <v>6.7813092361548713E-2</v>
       </c>
     </row>
-    <row r="378" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="378" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A378">
         <v>4000</v>
       </c>
@@ -9147,7 +9144,7 @@
         <v>6.5325357170343393E-2</v>
       </c>
     </row>
-    <row r="379" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="379" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A379">
         <v>4000</v>
       </c>
@@ -9159,7 +9156,7 @@
         <v>6.2928884981104827E-2</v>
       </c>
     </row>
-    <row r="380" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="380" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A380">
         <v>4000</v>
       </c>
@@ -9171,7 +9168,7 @@
         <v>6.062032779459358E-2</v>
       </c>
     </row>
-    <row r="381" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="381" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A381">
         <v>4000</v>
       </c>
@@ -9183,7 +9180,7 @@
         <v>5.8396460433509767E-2</v>
       </c>
     </row>
-    <row r="382" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="382" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A382">
         <v>4000</v>
       </c>
@@ -9195,7 +9192,7 @@
         <v>5.62541760367486E-2</v>
       </c>
     </row>
-    <row r="383" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="383" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A383">
         <v>4000</v>
       </c>
@@ -9207,7 +9204,7 @@
         <v>5.4190481718950051E-2</v>
       </c>
     </row>
-    <row r="384" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="384" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A384">
         <v>4000</v>
       </c>
@@ -9219,7 +9216,7 @@
         <v>5.2202494389278598E-2</v>
       </c>
     </row>
-    <row r="385" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="385" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A385">
         <v>4000</v>
       </c>
@@ -9231,7 +9228,7 @@
         <v>5.0287436723591865E-2</v>
       </c>
     </row>
-    <row r="386" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="386" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A386">
         <v>4000</v>
       </c>
@@ -9242,7 +9239,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="387" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="387" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A387">
         <v>4000</v>
       </c>
@@ -9253,7 +9250,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="388" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="388" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A388">
         <v>4000</v>
       </c>
@@ -9264,7 +9261,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="389" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="389" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A389">
         <v>4000</v>
       </c>
@@ -9275,7 +9272,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="390" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="390" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A390">
         <v>4000</v>
       </c>
@@ -9286,7 +9283,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="391" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="391" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A391">
         <v>4000</v>
       </c>
@@ -9297,7 +9294,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="392" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="392" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A392">
         <v>4000</v>
       </c>
@@ -9308,7 +9305,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="393" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="393" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A393">
         <v>4000</v>
       </c>
@@ -9319,7 +9316,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="394" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="394" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A394">
         <v>4000</v>
       </c>
@@ -9330,7 +9327,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="395" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="395" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A395">
         <v>4000</v>
       </c>
@@ -9341,7 +9338,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="396" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="396" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A396">
         <v>4000</v>
       </c>
@@ -9352,7 +9349,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="397" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="397" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A397">
         <v>4000</v>
       </c>
@@ -9363,7 +9360,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="398" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="398" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A398">
         <v>4000</v>
       </c>
@@ -9374,7 +9371,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="399" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="399" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A399">
         <v>4000</v>
       </c>
@@ -9385,7 +9382,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="400" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="400" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A400">
         <v>4000</v>
       </c>
@@ -9396,7 +9393,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="401" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="401" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A401">
         <v>4000</v>
       </c>
@@ -9407,7 +9404,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="402" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="402" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A402">
         <v>4000</v>
       </c>
@@ -9418,7 +9415,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="403" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="403" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A403">
         <v>4000</v>
       </c>
@@ -9429,7 +9426,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="404" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="404" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A404">
         <v>4000</v>
       </c>
@@ -9440,7 +9437,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="405" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="405" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A405">
         <v>4000</v>
       </c>
@@ -9451,7 +9448,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="406" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="406" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A406">
         <v>5000</v>
       </c>
@@ -9463,7 +9460,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="407" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="407" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A407">
         <v>5000</v>
       </c>
@@ -9475,7 +9472,7 @@
         <v>0.97054258295425244</v>
       </c>
     </row>
-    <row r="408" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="408" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A408">
         <v>5000</v>
       </c>
@@ -9487,7 +9484,7 @@
         <v>0.94195290532751197</v>
       </c>
     </row>
-    <row r="409" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="409" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A409">
         <v>5000</v>
       </c>
@@ -9499,7 +9496,7 @@
         <v>0.91420540575782594</v>
       </c>
     </row>
-    <row r="410" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="410" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A410">
         <v>5000</v>
       </c>
@@ -9511,7 +9508,7 @@
         <v>0.8872752758549407</v>
       </c>
     </row>
-    <row r="411" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="411" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A411">
         <v>5000</v>
       </c>
@@ -9523,7 +9520,7 @@
         <v>0.86113843801970102</v>
       </c>
     </row>
-    <row r="412" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="412" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A412">
         <v>5000</v>
       </c>
@@ -9535,7 +9532,7 @@
         <v>0.83577152391683107</v>
       </c>
     </row>
-    <row r="413" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="413" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A413">
         <v>5000</v>
       </c>
@@ -9547,7 +9544,7 @@
         <v>0.81115185358185304</v>
       </c>
     </row>
-    <row r="414" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="414" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A414">
         <v>5000</v>
       </c>
@@ -9559,7 +9556,7 @@
         <v>0.78725741514346115</v>
       </c>
     </row>
-    <row r="415" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="415" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A415">
         <v>5000</v>
       </c>
@@ -9571,7 +9568,7 @@
         <v>0.76406684514322298</v>
       </c>
     </row>
-    <row r="416" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="416" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A416">
         <v>5000</v>
       </c>
@@ -9583,7 +9580,7 @@
         <v>0.74155940943501053</v>
       </c>
     </row>
-    <row r="417" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="417" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A417">
         <v>5000</v>
       </c>
@@ -9595,7 +9592,7 @@
         <v>0.71971498464708517</v>
       </c>
     </row>
-    <row r="418" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="418" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A418">
         <v>5000</v>
       </c>
@@ -9607,7 +9604,7 @@
         <v>0.69851404019026209</v>
       </c>
     </row>
-    <row r="419" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="419" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A419">
         <v>5000</v>
       </c>
@@ -9619,7 +9616,7 @@
         <v>0.67793762079606756</v>
       </c>
     </row>
-    <row r="420" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="420" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A420">
         <v>5000</v>
       </c>
@@ -9631,7 +9628,7 @@
         <v>0.65796732956927584</v>
       </c>
     </row>
-    <row r="421" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="421" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A421">
         <v>5000</v>
       </c>
@@ -9643,7 +9640,7 @@
         <v>0.6385853115396769</v>
       </c>
     </row>
-    <row r="422" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="422" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A422">
         <v>5000</v>
       </c>
@@ -9655,7 +9652,7 @@
         <v>0.61977423769836404</v>
       </c>
     </row>
-    <row r="423" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="423" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A423">
         <v>5000</v>
       </c>
@@ -9667,7 +9664,7 @@
         <v>0.60151728950427308</v>
       </c>
     </row>
-    <row r="424" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="424" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A424">
         <v>5000</v>
       </c>
@@ -9679,7 +9676,7 @@
         <v>0.58379814384711792</v>
       </c>
     </row>
-    <row r="425" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="425" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A425">
         <v>5000</v>
       </c>
@@ -9691,7 +9688,7 @@
         <v>0.56660095845328007</v>
       </c>
     </row>
-    <row r="426" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="426" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A426">
         <v>5000</v>
       </c>
@@ -9703,7 +9700,7 @@
         <v>0.54991035772160157</v>
       </c>
     </row>
-    <row r="427" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="427" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A427">
         <v>5000</v>
       </c>
@@ -9715,7 +9712,7 @@
         <v>0.53371141897642005</v>
       </c>
     </row>
-    <row r="428" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="428" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A428">
         <v>5000</v>
       </c>
@@ -9727,7 +9724,7 @@
         <v>0.51798965912555395</v>
       </c>
     </row>
-    <row r="429" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="429" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A429">
         <v>5000</v>
       </c>
@@ -9739,7 +9736,7 @@
         <v>0.5027310217113079</v>
       </c>
     </row>
-    <row r="430" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="430" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A430">
         <v>5000</v>
       </c>
@@ -9751,7 +9748,7 @@
         <v>0.48792186434292317</v>
       </c>
     </row>
-    <row r="431" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="431" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A431">
         <v>5000</v>
       </c>
@@ -9763,7 +9760,7 @@
         <v>0.47354894649923496</v>
       </c>
     </row>
-    <row r="432" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="432" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A432">
         <v>5000</v>
       </c>
@@ -9775,7 +9772,7 @@
         <v>0.45959941769063267</v>
       </c>
     </row>
-    <row r="433" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="433" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A433">
         <v>5000</v>
       </c>
@@ -9787,7 +9784,7 @@
         <v>0.44606080596973696</v>
       </c>
     </row>
-    <row r="434" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="434" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A434">
         <v>5000</v>
       </c>
@@ -9799,7 +9796,7 @@
         <v>0.43292100678052409</v>
       </c>
     </row>
-    <row r="435" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="435" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A435">
         <v>5000</v>
       </c>
@@ -9811,7 +9808,7 @@
         <v>0.42016827213592534</v>
       </c>
     </row>
-    <row r="436" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="436" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A436">
         <v>5000</v>
       </c>
@@ -9823,7 +9820,7 @@
         <v>0.4077912001142262</v>
       </c>
     </row>
-    <row r="437" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="437" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A437">
         <v>5000</v>
       </c>
@@ -9835,7 +9832,7 @@
         <v>0.39577872466487551</v>
       </c>
     </row>
-    <row r="438" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="438" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A438">
         <v>5000</v>
       </c>
@@ -9847,7 +9844,7 @@
         <v>0.38412010571458821</v>
       </c>
     </row>
-    <row r="439" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="439" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A439">
         <v>5000</v>
       </c>
@@ -9859,7 +9856,7 @@
         <v>0.37280491956489692</v>
       </c>
     </row>
-    <row r="440" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="440" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A440">
         <v>5000</v>
       </c>
@@ -9871,7 +9868,7 @@
         <v>0.36182304957256745</v>
       </c>
     </row>
-    <row r="441" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="441" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A441">
         <v>5000</v>
       </c>
@@ -9883,7 +9880,7 @@
         <v>0.35116467710454408</v>
       </c>
     </row>
-    <row r="442" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="442" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A442">
         <v>5000</v>
       </c>
@@ -9895,7 +9892,7 @@
         <v>0.34082027275934024</v>
       </c>
     </row>
-    <row r="443" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="443" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A443">
         <v>5000</v>
       </c>
@@ -9907,7 +9904,7 @@
         <v>0.33078058784702291</v>
       </c>
     </row>
-    <row r="444" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="444" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A444">
         <v>5000</v>
       </c>
@@ -9919,7 +9916,7 @@
         <v>0.32103664612017563</v>
       </c>
     </row>
-    <row r="445" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="445" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A445">
         <v>5000</v>
       </c>
@@ -9931,7 +9928,7 @@
         <v>0.31157973574844561</v>
       </c>
     </row>
-    <row r="446" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="446" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A446">
         <v>5000</v>
       </c>
@@ -9943,7 +9940,7 @@
         <v>0.30240140152949979</v>
       </c>
     </row>
-    <row r="447" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="447" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A447">
         <v>5000</v>
       </c>
@@ -9955,7 +9952,7 @@
         <v>0.29349343732942673</v>
       </c>
     </row>
-    <row r="448" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="448" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A448">
         <v>5000</v>
       </c>
@@ -9967,7 +9964,7 @@
         <v>0.28484787874582385</v>
       </c>
     </row>
-    <row r="449" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="449" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A449">
         <v>5000</v>
       </c>
@@ -9979,7 +9976,7 @@
         <v>0.27645699598701157</v>
       </c>
     </row>
-    <row r="450" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="450" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A450">
         <v>5000</v>
       </c>
@@ -9991,7 +9988,7 @@
         <v>0.26831328696100759</v>
       </c>
     </row>
-    <row r="451" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="451" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A451">
         <v>5000</v>
       </c>
@@ -10003,7 +10000,7 @@
         <v>0.26040947056808189</v>
       </c>
     </row>
-    <row r="452" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="452" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A452">
         <v>5000</v>
       </c>
@@ -10015,7 +10012,7 @@
         <v>0.25273848019089556</v>
       </c>
     </row>
-    <row r="453" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="453" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A453">
         <v>5000</v>
       </c>
@@ -10027,7 +10024,7 @@
         <v>0.24529345737640393</v>
       </c>
     </row>
-    <row r="454" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="454" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A454">
         <v>5000</v>
       </c>
@@ -10039,7 +10036,7 @@
         <v>0.2380677457038739</v>
       </c>
     </row>
-    <row r="455" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="455" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A455">
         <v>5000</v>
       </c>
@@ -10051,7 +10048,7 @@
         <v>0.2310548848335339</v>
       </c>
     </row>
-    <row r="456" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="456" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A456">
         <v>5000</v>
       </c>
@@ -10063,7 +10060,7 @@
         <v>0.22424860473053532</v>
       </c>
     </row>
-    <row r="457" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="457" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A457">
         <v>5000</v>
       </c>
@@ -10075,7 +10072,7 @@
         <v>0.21764282005906097</v>
       </c>
     </row>
-    <row r="458" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="458" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A458">
         <v>5000</v>
       </c>
@@ -10087,7 +10084,7 @@
         <v>0.21123162474156862</v>
       </c>
     </row>
-    <row r="459" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="459" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A459">
         <v>5000</v>
       </c>
@@ -10099,7 +10096,7 @@
         <v>0.20500928667830537</v>
       </c>
     </row>
-    <row r="460" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="460" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A460">
         <v>5000</v>
       </c>
@@ -10111,7 +10108,7 @@
         <v>0.19897024262237131</v>
       </c>
     </row>
-    <row r="461" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="461" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A461">
         <v>5000</v>
       </c>
@@ -10123,7 +10120,7 @@
         <v>0.19310909320575054</v>
       </c>
     </row>
-    <row r="462" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="462" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A462">
         <v>5000</v>
       </c>
@@ -10135,7 +10132,7 @@
         <v>0.1874205981118626</v>
       </c>
     </row>
-    <row r="463" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="463" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A463">
         <v>5000</v>
       </c>
@@ -10147,7 +10144,7 @@
         <v>0.18189967139031804</v>
       </c>
     </row>
-    <row r="464" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="464" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A464">
         <v>5000</v>
       </c>
@@ -10159,7 +10156,7 @@
         <v>0.17654137690968899</v>
       </c>
     </row>
-    <row r="465" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="465" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A465">
         <v>5000</v>
       </c>
@@ -10171,7 +10168,7 @@
         <v>0.17134092394422978</v>
       </c>
     </row>
-    <row r="466" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="466" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A466">
         <v>5000</v>
       </c>
@@ -10183,7 +10180,7 @@
         <v>0.16629366289060088</v>
       </c>
     </row>
-    <row r="467" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="467" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A467">
         <v>5000</v>
       </c>
@@ -10195,7 +10192,7 @@
         <v>0.16139508111076747</v>
       </c>
     </row>
-    <row r="468" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="468" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A468">
         <v>5000</v>
       </c>
@@ -10207,7 +10204,7 @@
         <v>0.15664079889735535</v>
       </c>
     </row>
-    <row r="469" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="469" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A469">
         <v>5000</v>
       </c>
@@ -10219,7 +10216,7 @@
         <v>0.1520265655578569</v>
       </c>
     </row>
-    <row r="470" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="470" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A470">
         <v>5000</v>
       </c>
@@ -10231,7 +10228,7 @@
         <v>0.14754825561418644</v>
       </c>
     </row>
-    <row r="471" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="471" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A471">
         <v>5000</v>
       </c>
@@ -10243,7 +10240,7 @@
         <v>0.14320186511418675</v>
       </c>
     </row>
-    <row r="472" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="472" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A472">
         <v>5000</v>
       </c>
@@ -10255,7 +10252,7 @@
         <v>0.13898350805178927</v>
       </c>
     </row>
-    <row r="473" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="473" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A473">
         <v>5000</v>
       </c>
@@ -10267,7 +10264,7 @@
         <v>0.13488941289262674</v>
       </c>
     </row>
-    <row r="474" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="474" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A474">
         <v>5000</v>
       </c>
@@ -10279,7 +10276,7 @@
         <v>0.13091591920199258</v>
       </c>
     </row>
-    <row r="475" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="475" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A475">
         <v>5000</v>
       </c>
@@ -10291,7 +10288,7 @@
         <v>0.12705947437213208</v>
       </c>
     </row>
-    <row r="476" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="476" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A476">
         <v>5000</v>
       </c>
@@ -10303,7 +10300,7 @@
         <v>0.12331663044593871</v>
       </c>
     </row>
-    <row r="477" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="477" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A477">
         <v>5000</v>
       </c>
@@ -10315,7 +10312,7 @@
         <v>0.11968404103421637</v>
       </c>
     </row>
-    <row r="478" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="478" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A478">
         <v>5000</v>
       </c>
@@ -10327,7 +10324,7 @@
         <v>0.11615845832375109</v>
       </c>
     </row>
-    <row r="479" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="479" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A479">
         <v>5000</v>
       </c>
@@ -10339,7 +10336,7 @@
         <v>0.11273673017351726</v>
       </c>
     </row>
-    <row r="480" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="480" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A480">
         <v>5000</v>
       </c>
@@ -10351,7 +10348,7 @@
         <v>0.10941579729642205</v>
       </c>
     </row>
-    <row r="481" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="481" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A481">
         <v>5000</v>
       </c>
@@ -10363,7 +10360,7 @@
         <v>0.10619269052406835</v>
       </c>
     </row>
-    <row r="482" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="482" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A482">
         <v>5000</v>
       </c>
@@ -10375,7 +10372,7 @@
         <v>0.10306452815209087</v>
       </c>
     </row>
-    <row r="483" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="483" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A483">
         <v>5000</v>
       </c>
@@ -10387,7 +10384,7 @@
         <v>0.10002851336369153</v>
       </c>
     </row>
-    <row r="484" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="484" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A484">
         <v>5000</v>
       </c>
@@ -10399,7 +10396,7 @@
         <v>9.7081931729071175E-2</v>
       </c>
     </row>
-    <row r="485" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="485" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A485">
         <v>5000</v>
       </c>
@@ -10411,7 +10408,7 @@
         <v>9.4222148778521128E-2</v>
       </c>
     </row>
-    <row r="486" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="486" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A486">
         <v>5000</v>
       </c>
@@ -10423,7 +10420,7 @@
         <v>9.1446607647005754E-2</v>
       </c>
     </row>
-    <row r="487" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="487" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A487">
         <v>5000</v>
       </c>
@@ -10435,7 +10432,7 @@
         <v>8.8752826788129055E-2</v>
       </c>
     </row>
-    <row r="488" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="488" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A488">
         <v>5000</v>
       </c>
@@ -10447,7 +10444,7 @@
         <v>8.6138397755442145E-2</v>
       </c>
     </row>
-    <row r="489" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="489" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A489">
         <v>5000</v>
       </c>
@@ -10459,7 +10456,7 @@
         <v>8.3600983049107597E-2</v>
       </c>
     </row>
-    <row r="490" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="490" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A490">
         <v>5000</v>
       </c>
@@ -10471,7 +10468,7 @@
         <v>8.1138314025995556E-2</v>
       </c>
     </row>
-    <row r="491" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="491" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A491">
         <v>5000</v>
       </c>
@@ -10483,7 +10480,7 @@
         <v>7.8748188871342967E-2</v>
       </c>
     </row>
-    <row r="492" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="492" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A492">
         <v>5000</v>
       </c>
@@ -10495,7 +10492,7 @@
         <v>7.6428470630162518E-2</v>
       </c>
     </row>
-    <row r="493" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="493" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A493">
         <v>5000</v>
       </c>
@@ -10507,7 +10504,7 @@
         <v>7.417708529664116E-2</v>
       </c>
     </row>
-    <row r="494" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="494" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A494">
         <v>5000</v>
       </c>
@@ -10519,7 +10516,7 @@
         <v>7.1992019959820006E-2</v>
       </c>
     </row>
-    <row r="495" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="495" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A495">
         <v>5000</v>
       </c>
@@ -10531,7 +10528,7 @@
         <v>6.9871321003897799E-2</v>
       </c>
     </row>
-    <row r="496" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="496" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A496">
         <v>5000</v>
       </c>
@@ -10543,7 +10540,7 @@
         <v>6.7813092361548713E-2</v>
       </c>
     </row>
-    <row r="497" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="497" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A497">
         <v>5000</v>
       </c>
@@ -10555,7 +10552,7 @@
         <v>6.5815493818692769E-2</v>
       </c>
     </row>
-    <row r="498" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="498" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A498">
         <v>5000</v>
       </c>
@@ -10567,7 +10564,7 @@
         <v>6.3876739369203711E-2</v>
       </c>
     </row>
-    <row r="499" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="499" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A499">
         <v>5000</v>
       </c>
@@ -10579,7 +10576,7 @@
         <v>6.199509561808255E-2</v>
       </c>
     </row>
-    <row r="500" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="500" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A500">
         <v>5000</v>
       </c>
@@ -10591,7 +10588,7 @@
         <v>6.0168880231669698E-2</v>
       </c>
     </row>
-    <row r="501" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="501" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A501">
         <v>5000</v>
       </c>
@@ -10603,7 +10600,7 @@
         <v>5.8396460433509767E-2</v>
       </c>
     </row>
-    <row r="502" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="502" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A502">
         <v>5000</v>
       </c>
@@ -10615,7 +10612,7 @@
         <v>5.6676251544524367E-2</v>
       </c>
     </row>
-    <row r="503" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="503" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A503">
         <v>5000</v>
       </c>
@@ -10627,7 +10624,7 @@
         <v>5.5006715566187615E-2</v>
       </c>
     </row>
-    <row r="504" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="504" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A504">
         <v>5000</v>
       </c>
@@ -10639,7 +10636,7 @@
         <v>5.3386359805437614E-2</v>
       </c>
     </row>
-    <row r="505" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="505" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A505">
         <v>5000</v>
       </c>
@@ -10651,7 +10648,7 @@
         <v>5.1813735540094503E-2</v>
       </c>
     </row>
-    <row r="506" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="506" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A506">
         <v>5000</v>
       </c>
@@ -10663,7 +10660,7 @@
         <v>5.0287436723591865E-2</v>
       </c>
     </row>
-    <row r="507" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="507" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A507">
         <v>5000</v>
       </c>

</xml_diff>